<commit_message>
added new data to Negociado de la Policia
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/npprVDedad.xlsx
+++ b/data/Negociado_de_Policia/npprVDedad.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="2" r:id="rId1"/>
     <sheet name="2022" sheetId="3" r:id="rId2"/>
     <sheet name="2023" sheetId="4" r:id="rId3"/>
+    <sheet name="2024" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>Desconocida</t>
   </si>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,7 +414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -685,7 +688,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <f>SUM(B2:D2)</f>
+        <f t="shared" ref="E2:E15" si="0">SUM(B2:D2)</f>
         <v>7</v>
       </c>
     </row>
@@ -746,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <f>SUM(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
@@ -764,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f>SUM(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
@@ -782,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>904</v>
       </c>
     </row>
@@ -800,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>1135</v>
       </c>
     </row>
@@ -818,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>1022</v>
       </c>
     </row>
@@ -836,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>742</v>
       </c>
     </row>
@@ -854,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <f>SUM(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>598</v>
       </c>
     </row>
@@ -872,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <f>SUM(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
@@ -890,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <f>SUM(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>283</v>
       </c>
     </row>
@@ -908,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <f>SUM(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>235</v>
       </c>
     </row>
@@ -926,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <f>SUM(B13:D13)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
     </row>
@@ -944,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <f>SUM(B14:D14)</f>
+        <f t="shared" si="0"/>
         <v>252</v>
       </c>
     </row>
@@ -962,7 +965,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="1">
-        <f>SUM(B15:D15)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
@@ -975,14 +978,305 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E15" si="0">SUM(B2:D2)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>262</v>
+      </c>
+      <c r="C5" s="1">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>355</v>
+      </c>
+      <c r="C6" s="1">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>299</v>
+      </c>
+      <c r="C7" s="1">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>226</v>
+      </c>
+      <c r="C9" s="1">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>366</v>
+      </c>
+      <c r="C10" s="1">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>51</v>
+      </c>
+      <c r="C14" s="1">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -1010,17 +1304,17 @@
         <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2" s="1">
         <f>SUM(B2:D2)</f>
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,17 +1322,17 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(B3:D3)</f>
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,17 +1340,17 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
         <f>SUM(B4:D4)</f>
-        <v>43</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,17 +1358,17 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>262</v>
+        <v>1039</v>
       </c>
       <c r="C5" s="1">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
         <f>SUM(B5:D5)</f>
-        <v>301</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,17 +1376,17 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>355</v>
+        <v>1390</v>
       </c>
       <c r="C6" s="1">
-        <v>62</v>
+        <v>257</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <f>SUM(B6:D6)</f>
-        <v>417</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1100,17 +1394,17 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>299</v>
+        <v>1277</v>
       </c>
       <c r="C7" s="1">
-        <v>65</v>
+        <v>246</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <f>SUM(B7:D7)</f>
-        <v>364</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,17 +1412,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>186</v>
+        <v>991</v>
       </c>
       <c r="C8" s="1">
-        <v>49</v>
+        <v>254</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <f>SUM(B8:D8)</f>
-        <v>235</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,17 +1430,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>226</v>
+        <v>809</v>
       </c>
       <c r="C9" s="1">
-        <v>31</v>
+        <v>160</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
         <f>SUM(B9:D9)</f>
-        <v>257</v>
+        <v>970</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,17 +1448,17 @@
         <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>366</v>
+        <v>551</v>
       </c>
       <c r="C10" s="1">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
         <f>SUM(B10:D10)</f>
-        <v>403</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,17 +1466,17 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>84</v>
+        <v>384</v>
       </c>
       <c r="C11" s="1">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
         <f>SUM(B11:D11)</f>
-        <v>112</v>
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,17 +1484,17 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="C12" s="1">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
         <f>SUM(B12:D12)</f>
-        <v>74</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,17 +1502,17 @@
         <v>2</v>
       </c>
       <c r="B13" s="1">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="C13" s="1">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
         <f>SUM(B13:D13)</f>
-        <v>44</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,17 +1520,17 @@
         <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>51</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
         <f>SUM(B14:D14)</f>
-        <v>72</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,14 +1541,14 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <f>SUM(B15:D15)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>